<commit_message>
Added 4 channel op amp to restore mono and cleaned up repo
</commit_message>
<xml_diff>
--- a/bom/3bpv2-m bom alternate.xlsx
+++ b/bom/3bpv2-m bom alternate.xlsx
@@ -148,7 +148,7 @@
     <t xml:space="preserve">Vishay</t>
   </si>
   <si>
-    <t xml:space="preserve">R1, R12, R15, R19</t>
+    <t xml:space="preserve">R1, R15</t>
   </si>
   <si>
     <t xml:space="preserve">2.20k</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">CRCW06032K20FKEB</t>
   </si>
   <si>
-    <t xml:space="preserve">R10</t>
+    <t xml:space="preserve">R10, R43</t>
   </si>
   <si>
     <t xml:space="preserve">4.7k</t>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">KOA Speer</t>
   </si>
   <si>
-    <t xml:space="preserve">R11, R13, R14, R17, R18</t>
+    <t xml:space="preserve">R11, R14, R17</t>
   </si>
   <si>
     <t xml:space="preserve">RK73H1JTTDD75R0F</t>
@@ -205,7 +205,7 @@
     <t xml:space="preserve">AC0603FR-07210KL</t>
   </si>
   <si>
-    <t xml:space="preserve">R26, R27, R30, R33</t>
+    <t xml:space="preserve">R26, R27, R30, R33, R41, R42</t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
@@ -241,7 +241,7 @@
     <t xml:space="preserve">RK73H1JTTD3003F</t>
   </si>
   <si>
-    <t xml:space="preserve">R36, R37</t>
+    <t xml:space="preserve">R36, R37, R44</t>
   </si>
   <si>
     <t xml:space="preserve">RK73H1JTTD3300F</t>
@@ -253,7 +253,7 @@
     <t xml:space="preserve">RK73H1JTTD5110F </t>
   </si>
   <si>
-    <t xml:space="preserve">R41, R42, R6, R7, R8, R9</t>
+    <t xml:space="preserve">R6, R7, R8, R9</t>
   </si>
   <si>
     <t xml:space="preserve">1k</t>
@@ -265,10 +265,10 @@
     <t xml:space="preserve">U1</t>
   </si>
   <si>
-    <t xml:space="preserve">SOIC-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL972IDR</t>
+    <t xml:space="preserve">SOIC-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL974IDR</t>
   </si>
   <si>
     <t xml:space="preserve">Texas Instruments</t>
@@ -481,10 +481,10 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="41.87"/>
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>43</v>
@@ -738,7 +738,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>46</v>
@@ -761,7 +761,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>75</v>
@@ -853,7 +853,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>62</v>
@@ -945,7 +945,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>330</v>
@@ -991,7 +991,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>78</v>

</xml_diff>